<commit_message>
completed part 3 and 4
</commit_message>
<xml_diff>
--- a/Upload Data/Listening Exercise/Part 3/Test 1/Test.xlsx
+++ b/Upload Data/Listening Exercise/Part 3/Test 1/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toan\git\PBL5-LPToeic\Upload Data\Listening Exercise\Part 3\Test 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701DF56B-96EF-4CF7-9201-E9BA2DBCE178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246D17AC-D228-4137-8238-0D0A4180B2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>Audio</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Đáp án A</t>
   </si>
@@ -43,9 +40,6 @@
   </si>
   <si>
     <t>Đáp án</t>
-  </si>
-  <si>
-    <t>cau1.mp3</t>
   </si>
   <si>
     <t>A</t>
@@ -146,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -208,52 +202,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -547,18 +506,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,82 +533,71 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="56" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F2" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="70">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="56" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="9" t="s">
+    <row r="4" spans="1:6" ht="56">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="70">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="56">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>